<commit_message>
Intégration du remplissage de la feuille Recapitulatif Excel avec les données des pointages.
</commit_message>
<xml_diff>
--- a/Symfony/web/test.xlsx
+++ b/Symfony/web/test.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Absences" sheetId="1" r:id="rId4"/>
+    <sheet name="Absence" sheetId="1" r:id="rId4"/>
     <sheet name="Totaux" sheetId="2" r:id="rId5"/>
-    <sheet name="Worksheet" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>Nom/Prénom</t>
   </si>
@@ -32,6 +31,132 @@
   </si>
   <si>
     <t>Commentaires</t>
+  </si>
+  <si>
+    <t>BESSON Tristan</t>
+  </si>
+  <si>
+    <t>01-09-2016</t>
+  </si>
+  <si>
+    <t>02-09-2016</t>
+  </si>
+  <si>
+    <t>03-09-2016</t>
+  </si>
+  <si>
+    <t>04-09-2016</t>
+  </si>
+  <si>
+    <t>05-09-2016</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>06-09-2016</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Malade</t>
+  </si>
+  <si>
+    <t>07-09-2016</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>08-09-2016</t>
+  </si>
+  <si>
+    <t>Accident</t>
+  </si>
+  <si>
+    <t>09-09-2016</t>
+  </si>
+  <si>
+    <t>10-09-2016</t>
+  </si>
+  <si>
+    <t>11-09-2016</t>
+  </si>
+  <si>
+    <t>12-09-2016</t>
+  </si>
+  <si>
+    <t>13-09-2016</t>
+  </si>
+  <si>
+    <t>14-09-2016</t>
+  </si>
+  <si>
+    <t>15-09-2016</t>
+  </si>
+  <si>
+    <t>16-09-2016</t>
+  </si>
+  <si>
+    <t>17-09-2016</t>
+  </si>
+  <si>
+    <t>18-09-2016</t>
+  </si>
+  <si>
+    <t>19-09-2016</t>
+  </si>
+  <si>
+    <t>20-09-2016</t>
+  </si>
+  <si>
+    <t>21-09-2016</t>
+  </si>
+  <si>
+    <t>22-09-2016</t>
+  </si>
+  <si>
+    <t>23-09-2016</t>
+  </si>
+  <si>
+    <t>24-09-2016</t>
+  </si>
+  <si>
+    <t>25-09-2016</t>
+  </si>
+  <si>
+    <t>26-09-2016</t>
+  </si>
+  <si>
+    <t>27-09-2016</t>
+  </si>
+  <si>
+    <t>28-09-2016</t>
+  </si>
+  <si>
+    <t>29-09-2016</t>
+  </si>
+  <si>
+    <t>30-09-2016</t>
+  </si>
+  <si>
+    <t>MORISSEAU Laurent</t>
+  </si>
+  <si>
+    <t>POUZOLS Arnaud</t>
+  </si>
+  <si>
+    <t>Titre repas</t>
+  </si>
+  <si>
+    <t>Forfaits déplacement</t>
+  </si>
+  <si>
+    <t>Primes panier</t>
+  </si>
+  <si>
+    <t>Titre transport</t>
   </si>
 </sst>
 </file>
@@ -39,7 +164,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -49,8 +174,17 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -60,6 +194,9 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -67,9 +204,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+  <cellXfs count="4">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="14" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -370,14 +516,1052 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="true" style="0"/>
+    <col min="3" max="3" width="14" customWidth="true" style="0"/>
+    <col min="4" max="4" width="18.28515625" customWidth="true" style="0"/>
+    <col min="5" max="5" width="34.28515625" customWidth="true" style="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="E52"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56" t="s">
+        <v>35</v>
+      </c>
+      <c r="E56"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" t="s">
+        <v>39</v>
+      </c>
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="E60"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" t="s">
+        <v>40</v>
+      </c>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="E62"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="E63"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64"/>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65"/>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>42</v>
+      </c>
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66"/>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>42</v>
+      </c>
+      <c r="B67" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>42</v>
+      </c>
+      <c r="B68" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" t="s">
+        <v>16</v>
+      </c>
+      <c r="D68" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68"/>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>42</v>
+      </c>
+      <c r="B69" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" t="s">
+        <v>16</v>
+      </c>
+      <c r="D69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" t="s">
+        <v>16</v>
+      </c>
+      <c r="D70" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70"/>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" t="s">
+        <v>20</v>
+      </c>
+      <c r="E71"/>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>42</v>
+      </c>
+      <c r="B72" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72"/>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>42</v>
+      </c>
+      <c r="B73" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73"/>
+      <c r="D73"/>
+      <c r="E73"/>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>42</v>
+      </c>
+      <c r="B74" t="s">
+        <v>23</v>
+      </c>
+      <c r="C74"/>
+      <c r="D74"/>
+      <c r="E74"/>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>42</v>
+      </c>
+      <c r="B75" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75"/>
+      <c r="D75"/>
+      <c r="E75"/>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>42</v>
+      </c>
+      <c r="B76" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76"/>
+      <c r="D76"/>
+      <c r="E76"/>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>42</v>
+      </c>
+      <c r="B77" t="s">
+        <v>26</v>
+      </c>
+      <c r="C77"/>
+      <c r="D77"/>
+      <c r="E77"/>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>42</v>
+      </c>
+      <c r="B78" t="s">
+        <v>27</v>
+      </c>
+      <c r="E78"/>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>42</v>
+      </c>
+      <c r="B79" t="s">
+        <v>28</v>
+      </c>
+      <c r="E79"/>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80" t="s">
+        <v>29</v>
+      </c>
+      <c r="C80"/>
+      <c r="D80"/>
+      <c r="E80"/>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>42</v>
+      </c>
+      <c r="B81" t="s">
+        <v>30</v>
+      </c>
+      <c r="C81"/>
+      <c r="D81"/>
+      <c r="E81"/>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>42</v>
+      </c>
+      <c r="B82" t="s">
+        <v>31</v>
+      </c>
+      <c r="C82"/>
+      <c r="D82"/>
+      <c r="E82"/>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>42</v>
+      </c>
+      <c r="B83" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83"/>
+      <c r="D83"/>
+      <c r="E83"/>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>42</v>
+      </c>
+      <c r="B84" t="s">
+        <v>33</v>
+      </c>
+      <c r="C84"/>
+      <c r="D84"/>
+      <c r="E84"/>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>42</v>
+      </c>
+      <c r="B85" t="s">
+        <v>34</v>
+      </c>
+      <c r="E85"/>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>42</v>
+      </c>
+      <c r="B86" t="s">
+        <v>35</v>
+      </c>
+      <c r="E86"/>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>42</v>
+      </c>
+      <c r="B87" t="s">
+        <v>36</v>
+      </c>
+      <c r="C87"/>
+      <c r="D87"/>
+      <c r="E87"/>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>42</v>
+      </c>
+      <c r="B88" t="s">
+        <v>37</v>
+      </c>
+      <c r="C88"/>
+      <c r="D88"/>
+      <c r="E88"/>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>42</v>
+      </c>
+      <c r="B89" t="s">
+        <v>38</v>
+      </c>
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="E89"/>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>42</v>
+      </c>
+      <c r="B90" t="s">
+        <v>39</v>
+      </c>
+      <c r="C90"/>
+      <c r="D90"/>
+      <c r="E90"/>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>42</v>
+      </c>
+      <c r="B91" t="s">
+        <v>40</v>
+      </c>
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="E91"/>
+    </row>
+  </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -398,57 +1582,87 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="true" style="0"/>
+    <col min="2" max="2" width="10.42578125" customWidth="true" style="0"/>
+    <col min="3" max="3" width="20.140625" customWidth="true" style="0"/>
+    <col min="4" max="4" width="13.28515625" customWidth="true" style="0"/>
+    <col min="5" max="5" width="13.85546875" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>